<commit_message>
mileage manager pagination feature fin
</commit_message>
<xml_diff>
--- a/SpringBoot/src/main/resources/static/mileScore/20240716 MonthlyBase.xlsx
+++ b/SpringBoot/src/main/resources/static/mileScore/20240716 MonthlyBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a769109cc77918e/바탕 화면/최종프로젝트/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C946655-E5C9-482B-8E51-D8E381A5F5D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{7AE3EFA4-6AF9-4DC3-9382-6429998DA279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC192759-CB60-4D5F-87E4-5E9E7A1F6C54}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{95B3ECED-501D-47D2-BEE2-B593F83AB676}"/>
   </bookViews>
@@ -98,7 +98,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -112,9 +112,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -434,7 +431,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -448,8 +445,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5">
-        <v>20240716</v>
+      <c r="A1" s="4">
+        <v>45489</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>